<commit_message>
VGA proper rewrite, empty output for now
</commit_message>
<xml_diff>
--- a/SCRIPTS/ShakeGenerator.xlsx
+++ b/SCRIPTS/ShakeGenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marosm\Documents\ISE_projects\MikroLode\SCRIPTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59D2CEBF-8D37-48CA-91AD-669F9578F9EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9EB9B0-53D2-45D4-BF5B-AF945CD1A0E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BC9B79BB-3677-476D-975D-74E8945B760E}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>Raw</t>
   </si>
   <si>
-    <t>Corrected</t>
-  </si>
-  <si>
     <t>Max:</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
   </si>
   <si>
     <t>std dev</t>
-  </si>
-  <si>
-    <t>Rounded</t>
   </si>
   <si>
     <t>Rand part</t>
@@ -74,13 +68,19 @@
   <si>
     <t>Hex</t>
   </si>
+  <si>
+    <t>Scaled ND</t>
+  </si>
+  <si>
+    <t>Rounded output</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -130,7 +130,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -183,7 +183,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Distribution</a:t>
+              <a:t>Random shake generator [preview]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -224,303 +224,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hárok1!$J$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Scale</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hárok1!$F$6:$F$65</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="60"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>52</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>57</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>58</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>59</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>60</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hárok1!$J$6:$J$24</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>-1.108877071032067</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.4540142555604545</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-10.862740408020542</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.9661925274669585</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-9.8201866391186421</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.958720230053764</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1.7035756478361623</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1.9221832657188709</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.4079384644891597</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-10.377630246279715</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.0520067458437004</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-6.4036667486838326</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.4103522823168189</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.55994919553866751</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-0.11368208225488739</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.18080303995554775</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-0.34596516462857607</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-0.4740299779586169</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.27589824283055647</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0724-4B19-AA60-C1AF3344A12B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Hárok1!$K$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Rounded</c:v>
+                  <c:v>Rounded output</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -736,58 +448,58 @@
                   <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>-11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-10</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -947,7 +659,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Corrected</c:v>
+                  <c:v>Scaled ND</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1380,6 +1092,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sample</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1419,7 +1186,7 @@
         </c:txPr>
         <c:crossAx val="1491359280"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
         <c:noMultiLvlLbl val="0"/>
@@ -1447,7 +1214,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Amplitude</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1492,7 +1314,67 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Scaled</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Normal Distribution</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1539,6 +1421,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1491374672"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1554,10 +1437,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:legendEntry>
-        <c:idx val="0"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2187,13 +2066,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>28574</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>190499</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2520,8 +2399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA1BE20-99CF-4314-8008-03FDC769839A}">
   <dimension ref="B2:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="K3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,7 +2418,7 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -2565,7 +2444,7 @@
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I4">
         <f>MAX(G:G)</f>
@@ -2574,13 +2453,13 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>0.2</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -2589,25 +2468,25 @@
         <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s">
         <v>10</v>
-      </c>
-      <c r="K5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E6" s="3">
         <f ca="1">2*(RAND()-0.5)</f>
-        <v>-0.12378106649005316</v>
+        <v>-0.13405339384489978</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -2622,11 +2501,11 @@
       </c>
       <c r="I6" s="3">
         <f ca="1">H6*E6</f>
-        <v>-6.9304816939504188E-2</v>
+        <v>-7.505627624630791E-2</v>
       </c>
       <c r="J6" s="3">
         <f ca="1">I6*$C$4</f>
-        <v>-1.108877071032067</v>
+        <v>-1.2009004199409266</v>
       </c>
       <c r="K6">
         <f ca="1">ROUND(J6, 0)</f>
@@ -2640,7 +2519,7 @@
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E7" s="3">
         <f t="shared" ref="E7:E65" ca="1" si="0">2*(RAND()-0.5)</f>
-        <v>0.40869629540548003</v>
+        <v>0.77122891276497119</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -2655,25 +2534,25 @@
       </c>
       <c r="I7" s="3">
         <f t="shared" ref="I7:I65" ca="1" si="3">H7*E7</f>
-        <v>0.27837589097252841</v>
+        <v>0.52530825003373527</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ref="J7:J65" ca="1" si="4">I7*$C$4</f>
-        <v>4.4540142555604545</v>
+        <v>8.4049320005397643</v>
       </c>
       <c r="K7">
         <f t="shared" ref="K7:K65" ca="1" si="5">ROUND(J7, 0)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L7" s="2" t="str">
         <f t="shared" ref="L7:L37" ca="1" si="6">RIGHT(DEC2HEX(K7,2), 1)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.85278305128097243</v>
+        <v>3.9546239867743083E-2</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -2688,25 +2567,25 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.67892127550128389</v>
+        <v>3.1483720943982267E-2</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-10.862740408020542</v>
+        <v>0.50373953510371627</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="5"/>
-        <v>-11</v>
+        <v>1</v>
       </c>
       <c r="L8" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48698599573132539</v>
+        <v>0.54940100106653178</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -2721,25 +2600,25 @@
       </c>
       <c r="I9" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.43538703296668491</v>
+        <v>0.49118881006848031</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>6.9661925274669585</v>
+        <v>7.8590209610956849</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L9" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.63625961831714961</v>
+        <v>-0.72417774555950731</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -2754,25 +2633,25 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.61376166494491513</v>
+        <v>-0.69857103301046963</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-9.8201866391186421</v>
+        <v>-11.177136528167514</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="5"/>
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="L10" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74742001437836025</v>
+        <v>-0.14898457403563881</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -2787,25 +2666,25 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.74742001437836025</v>
+        <v>-0.14898457403563881</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>11.958720230053764</v>
+        <v>-2.3837531845702209</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>-2</v>
       </c>
       <c r="L11" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>C</v>
+        <v>E</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.10690022482639683</v>
+        <v>3.252317482634659E-2</v>
       </c>
       <c r="F12">
         <v>7</v>
@@ -2820,25 +2699,25 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.10647347798976015</v>
+        <v>3.2393341965872589E-2</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.7035756478361623</v>
+        <v>0.51829347145396143</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="5"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="L12" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>E</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.12604364228424991</v>
+        <v>0.48195220742462053</v>
       </c>
       <c r="F13">
         <v>8</v>
@@ -2853,25 +2732,25 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.12013645410742943</v>
+        <v>0.45936493265299166</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.9221832657188709</v>
+        <v>7.3498389224478666</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="5"/>
-        <v>-2</v>
+        <v>7</v>
       </c>
       <c r="L13" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>E</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67096730306142471</v>
+        <v>0.99016238630171327</v>
       </c>
       <c r="F14">
         <v>9</v>
@@ -2886,25 +2765,25 @@
       </c>
       <c r="I14" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.58799615403057248</v>
+        <v>0.86771989090181034</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>9.4079384644891597</v>
+        <v>13.883518254428965</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="L14" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>E</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.8378332612613375</v>
+        <v>0.35990017183826617</v>
       </c>
       <c r="F15">
         <v>10</v>
@@ -2919,25 +2798,25 @@
       </c>
       <c r="I15" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.64860189039248217</v>
+        <v>0.27861382759554393</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-10.377630246279715</v>
+        <v>4.4578212415287028</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="5"/>
-        <v>-10</v>
+        <v>4</v>
       </c>
       <c r="L15" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10006961396409841</v>
+        <v>-6.0198861336815179E-2</v>
       </c>
       <c r="F16">
         <v>11</v>
@@ -2952,25 +2831,25 @@
       </c>
       <c r="I16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>6.5750421615231272E-2</v>
+        <v>-3.9553470397841996E-2</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>1.0520067458437004</v>
+        <v>-0.63285552636547193</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="L16" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>F</v>
       </c>
     </row>
     <row r="17" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.74697917945465986</v>
+        <v>9.5880406807071772E-3</v>
       </c>
       <c r="F17">
         <v>12</v>
@@ -2985,25 +2864,25 @@
       </c>
       <c r="I17" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-0.40022917179273954</v>
+        <v>5.1372430267147108E-3</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-6.4036667486838326</v>
+        <v>8.2195888427435373E-2</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="5"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
       <c r="L17" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>A</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E18" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50774642080092902</v>
+        <v>-0.75802985513768184</v>
       </c>
       <c r="F18">
         <v>13</v>
@@ -3018,25 +2897,25 @@
       </c>
       <c r="I18" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>0.21314701764480118</v>
+        <v>-0.31821357332948025</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3.4103522823168189</v>
+        <v>-5.091417173271684</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="L18" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>B</v>
       </c>
     </row>
     <row r="19" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11074799834432647</v>
+        <v>0.66176772813499074</v>
       </c>
       <c r="F19">
         <v>14</v>
@@ -3051,25 +2930,25 @@
       </c>
       <c r="I19" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>3.4996824721166719E-2</v>
+        <v>0.20912133432569111</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.55994919553866751</v>
+        <v>3.3459413492110577</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L19" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.1087850328912259E-2</v>
+        <v>-0.33668044554497945</v>
       </c>
       <c r="F20">
         <v>15</v>
@@ -3084,25 +2963,25 @@
       </c>
       <c r="I20" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-7.105130140930462E-3</v>
+        <v>-7.694833692887347E-2</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.11368208225488739</v>
+        <v>-1.2311733908619755</v>
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L20" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>F</v>
       </c>
     </row>
     <row r="21" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1152078674377339E-2</v>
+        <v>-0.31601039213123006</v>
       </c>
       <c r="F21">
         <v>16</v>
@@ -3117,25 +2996,25 @@
       </c>
       <c r="I21" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1.1300189997221734E-2</v>
+        <v>-5.0187957101320672E-2</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.18080303995554775</v>
+        <v>-0.80300731362113076</v>
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L21" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>F</v>
       </c>
     </row>
     <row r="22" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.20392440623212993</v>
+        <v>-0.44881483439144443</v>
       </c>
       <c r="F22">
         <v>17</v>
@@ -3150,25 +3029,25 @@
       </c>
       <c r="I22" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-2.1622822789286004E-2</v>
+        <v>-4.7589417120587424E-2</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.34596516462857607</v>
+        <v>-0.76143067392939878</v>
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L22" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>F</v>
       </c>
     </row>
     <row r="23" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.43558146606517667</v>
+        <v>-0.20952574975946581</v>
       </c>
       <c r="F23">
         <v>18</v>
@@ -3183,11 +3062,11 @@
       </c>
       <c r="I23" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-2.9626873622413556E-2</v>
+        <v>-1.4251278790260304E-2</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.4740299779586169</v>
+        <v>-0.22802046064416487</v>
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="5"/>
@@ -3201,7 +3080,7 @@
     <row r="24" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E24" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4113495707502155</v>
+        <v>-0.7590200895543564</v>
       </c>
       <c r="F24">
         <v>19</v>
@@ -3216,25 +3095,25 @@
       </c>
       <c r="I24" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1.724364017690978E-2</v>
+        <v>-3.1817875213655616E-2</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.27589824283055647</v>
+        <v>-0.50908600341848986</v>
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="L24" s="2" t="str">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>F</v>
       </c>
     </row>
     <row r="25" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E25" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47758303642575362</v>
+        <v>-0.63281624651116797</v>
       </c>
       <c r="F25">
         <v>20</v>
@@ -3249,11 +3128,11 @@
       </c>
       <c r="I25" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1.185486157659647E-2</v>
+        <v>-1.5708156349011192E-2</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.18967778522554352</v>
+        <v>-0.25133050158417908</v>
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="5"/>
@@ -3267,7 +3146,7 @@
     <row r="26" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E26" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.58956997803334144</v>
+        <v>-0.93052470957726752</v>
       </c>
       <c r="F26">
         <v>21</v>
@@ -3282,11 +3161,11 @@
       </c>
       <c r="I26" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>8.3260855217405748E-3</v>
+        <v>-1.314115134878017E-2</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>0.1332173683478492</v>
+        <v>-0.21025842158048272</v>
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="5"/>
@@ -3298,13 +3177,13 @@
       </c>
       <c r="M26" t="str">
         <f ca="1">"x"&amp;CHAR(34)&amp;_xlfn.TEXTJOIN(CHAR(34)&amp;",x"&amp;CHAR(34),TRUE,L6:INDIRECT(CONCATENATE("L",$D$3)))&amp;CHAR(34)</f>
-        <v>x"F",x"4",x"5",x"7",x"6",x"C",x"E",x"E",x"9",x"6",x"1",x"A",x"3",x"1",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0"</v>
+        <v>x"F",x"8",x"1",x"8",x"5",x"E",x"1",x"7",x"E",x"4",x"F",x"0",x"B",x"3",x"F",x"F",x"F",x"0",x"F",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0",x"0"</v>
       </c>
     </row>
     <row r="27" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E27" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17789738317189441</v>
+        <v>-0.80456504540235629</v>
       </c>
       <c r="F27">
         <v>22</v>
@@ -3319,11 +3198,11 @@
       </c>
       <c r="I27" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1.3732866549729563E-3</v>
+        <v>-6.2108751697665613E-3</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>2.1972586479567301E-2</v>
+        <v>-9.9374002716264981E-2</v>
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="5"/>
@@ -3337,7 +3216,7 @@
     <row r="28" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E28" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49262303982320677</v>
+        <v>0.70836616511102513</v>
       </c>
       <c r="F28">
         <v>23</v>
@@ -3352,11 +3231,11 @@
       </c>
       <c r="I28" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>1.9971961190815607E-3</v>
+        <v>2.8718635578964258E-3</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>3.1955137905304971E-2</v>
+        <v>4.5949816926342812E-2</v>
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="5"/>
@@ -3370,7 +3249,7 @@
     <row r="29" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E29" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.68164364974000957</v>
+        <v>-0.91870678184391008</v>
       </c>
       <c r="F29">
         <v>24</v>
@@ -3385,11 +3264,11 @@
       </c>
       <c r="I29" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-1.3944596792997575E-3</v>
+        <v>-1.8794271242300934E-3</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.231135486879612E-2</v>
+        <v>-3.0070833987681494E-2</v>
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="5"/>
@@ -3403,7 +3282,7 @@
     <row r="30" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E30" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.2908250508456891</v>
+        <v>-0.66328244191408303</v>
       </c>
       <c r="F30">
         <v>25</v>
@@ -3418,11 +3297,11 @@
       </c>
       <c r="I30" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-2.884371368056051E-4</v>
+        <v>-6.5783634484994729E-4</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-4.6149941888896815E-3</v>
+        <v>-1.0525381517599157E-2</v>
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="5"/>
@@ -3436,7 +3315,7 @@
     <row r="31" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E31" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87624920182161059</v>
+        <v>-3.4716544534124427E-2</v>
       </c>
       <c r="F31">
         <v>26</v>
@@ -3451,11 +3330,11 @@
       </c>
       <c r="I31" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>4.0480513631904074E-4</v>
+        <v>-1.6038172147200803E-5</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>6.4768821811046519E-3</v>
+        <v>-2.5661075435521284E-4</v>
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="5"/>
@@ -3469,7 +3348,7 @@
     <row r="32" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E32" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.21942793606524957</v>
+        <v>0.63127964533532044</v>
       </c>
       <c r="F32">
         <v>27</v>
@@ -3484,11 +3363,11 @@
       </c>
       <c r="I32" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.5366735946381567E-5</v>
+        <v>1.3051709591679658E-4</v>
       </c>
       <c r="J32" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-7.2586777514210507E-4</v>
+        <v>2.0882735346687453E-3</v>
       </c>
       <c r="K32">
         <f t="shared" ca="1" si="5"/>
@@ -3502,7 +3381,7 @@
     <row r="33" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E33" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.43007363502705176</v>
+        <v>-0.85913447419517541</v>
       </c>
       <c r="F33">
         <v>28</v>
@@ -3517,11 +3396,11 @@
       </c>
       <c r="I33" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-3.8233485570773787E-5</v>
+        <v>-7.6376933732358253E-5</v>
       </c>
       <c r="J33" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-6.1173576913238058E-4</v>
+        <v>-1.222030939717732E-3</v>
       </c>
       <c r="K33">
         <f t="shared" ca="1" si="5"/>
@@ -3535,7 +3414,7 @@
     <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E34" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.24867706064973039</v>
+        <v>-0.96573551055321571</v>
       </c>
       <c r="F34">
         <v>29</v>
@@ -3550,11 +3429,11 @@
       </c>
       <c r="I34" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-9.1331475977260813E-6</v>
+        <v>-3.5468510586392265E-5</v>
       </c>
       <c r="J34" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.461303615636173E-4</v>
+        <v>-5.6749616938227623E-4</v>
       </c>
       <c r="K34">
         <f t="shared" ca="1" si="5"/>
@@ -3568,7 +3447,7 @@
     <row r="35" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E35" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.50005562001662751</v>
+        <v>-0.18507015640326552</v>
       </c>
       <c r="F35">
         <v>30</v>
@@ -3583,11 +3462,11 @@
       </c>
       <c r="I35" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-7.2897890685805342E-6</v>
+        <v>-2.6979446866813628E-6</v>
       </c>
       <c r="J35" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.1663662509728855E-4</v>
+        <v>-4.3167114986901804E-5</v>
       </c>
       <c r="K35">
         <f t="shared" ca="1" si="5"/>
@@ -3601,7 +3480,7 @@
     <row r="36" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E36" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.80325797487046913</v>
+        <v>-0.98724145611519787</v>
       </c>
       <c r="F36">
         <v>31</v>
@@ -3616,11 +3495,11 @@
       </c>
       <c r="I36" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-4.4657233477534548E-6</v>
+        <v>-5.4885819479784155E-6</v>
       </c>
       <c r="J36" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-7.1451573564055277E-5</v>
+        <v>-8.7817311167654648E-5</v>
       </c>
       <c r="K36">
         <f t="shared" ca="1" si="5"/>
@@ -3634,7 +3513,7 @@
     <row r="37" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E37" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.6261845914240014</v>
+        <v>-0.50163000173590588</v>
       </c>
       <c r="F37">
         <v>32</v>
@@ -3649,11 +3528,11 @@
       </c>
       <c r="I37" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>-1.2755793672613151E-6</v>
+        <v>-1.021853442222937E-6</v>
       </c>
       <c r="J37" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.0409269876181041E-5</v>
+        <v>-1.6349655075566991E-5</v>
       </c>
       <c r="K37">
         <f t="shared" ca="1" si="5"/>
@@ -3667,7 +3546,7 @@
     <row r="38" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E38" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1114614471688977E-3</v>
+        <v>-0.8616025038773214</v>
       </c>
       <c r="F38">
         <v>33</v>
@@ -3696,7 +3575,7 @@
     <row r="39" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E39" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66809755433886209</v>
+        <v>8.8329536660719743E-2</v>
       </c>
       <c r="F39">
         <v>34</v>
@@ -3725,7 +3604,7 @@
     <row r="40" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E40" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88749677763217116</v>
+        <v>-0.19209676466769277</v>
       </c>
       <c r="F40">
         <v>35</v>
@@ -3754,7 +3633,7 @@
     <row r="41" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E41" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.81070150480250436</v>
+        <v>3.5791950160234842E-2</v>
       </c>
       <c r="F41">
         <v>36</v>
@@ -3783,7 +3662,7 @@
     <row r="42" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E42" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76653741229674655</v>
+        <v>-0.94796733890137208</v>
       </c>
       <c r="F42">
         <v>37</v>
@@ -3812,7 +3691,7 @@
     <row r="43" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E43" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55488585925945766</v>
+        <v>-0.35891641558128784</v>
       </c>
       <c r="F43">
         <v>38</v>
@@ -3841,7 +3720,7 @@
     <row r="44" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E44" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86799906700804574</v>
+        <v>-0.98523829578291799</v>
       </c>
       <c r="F44">
         <v>39</v>
@@ -3870,7 +3749,7 @@
     <row r="45" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E45" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.96899209312315993</v>
+        <v>-0.27090199384339408</v>
       </c>
       <c r="F45">
         <v>40</v>
@@ -3899,7 +3778,7 @@
     <row r="46" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E46" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.88572840189473445</v>
+        <v>-0.91258943140667381</v>
       </c>
       <c r="F46">
         <v>41</v>
@@ -3928,7 +3807,7 @@
     <row r="47" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E47" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.37780238287794554</v>
+        <v>0.38211136675864221</v>
       </c>
       <c r="F47">
         <v>42</v>
@@ -3957,7 +3836,7 @@
     <row r="48" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E48" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.39117010705441246</v>
+        <v>-0.32960722096950135</v>
       </c>
       <c r="F48">
         <v>43</v>
@@ -3986,7 +3865,7 @@
     <row r="49" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E49" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.26097274736140719</v>
+        <v>0.98639402919057217</v>
       </c>
       <c r="F49">
         <v>44</v>
@@ -4015,7 +3894,7 @@
     <row r="50" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E50" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73968866071080597</v>
+        <v>0.66101275385530944</v>
       </c>
       <c r="F50">
         <v>45</v>
@@ -4044,7 +3923,7 @@
     <row r="51" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E51" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48586090721689223</v>
+        <v>-0.81519896956918148</v>
       </c>
       <c r="F51">
         <v>46</v>
@@ -4073,7 +3952,7 @@
     <row r="52" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E52" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.54834073674966932</v>
+        <v>0.2207840357374018</v>
       </c>
       <c r="F52">
         <v>47</v>
@@ -4102,7 +3981,7 @@
     <row r="53" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E53" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23479178298061165</v>
+        <v>0.39036666652295415</v>
       </c>
       <c r="F53">
         <v>48</v>
@@ -4131,7 +4010,7 @@
     <row r="54" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E54" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.45742076685320399</v>
+        <v>-8.3499782251869492E-2</v>
       </c>
       <c r="F54">
         <v>49</v>
@@ -4160,7 +4039,7 @@
     <row r="55" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E55" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57964582930700415</v>
+        <v>0.86798973807979984</v>
       </c>
       <c r="F55">
         <v>50</v>
@@ -4189,7 +4068,7 @@
     <row r="56" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E56" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.69538274693793145</v>
+        <v>6.7737176327651305E-2</v>
       </c>
       <c r="F56">
         <v>51</v>
@@ -4218,7 +4097,7 @@
     <row r="57" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E57" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.11239158782464398</v>
+        <v>-0.82590924666763965</v>
       </c>
       <c r="F57">
         <v>52</v>
@@ -4247,7 +4126,7 @@
     <row r="58" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E58" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21427067581309789</v>
+        <v>-0.86171488135882424</v>
       </c>
       <c r="F58">
         <v>53</v>
@@ -4276,7 +4155,7 @@
     <row r="59" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E59" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34471953926902077</v>
+        <v>-0.51855401355360731</v>
       </c>
       <c r="F59">
         <v>54</v>
@@ -4305,7 +4184,7 @@
     <row r="60" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E60" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.31336488623888803</v>
+        <v>0.35250924968398878</v>
       </c>
       <c r="F60">
         <v>55</v>
@@ -4334,7 +4213,7 @@
     <row r="61" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E61" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.10199348759973237</v>
+        <v>-5.3058333362663301E-2</v>
       </c>
       <c r="F61">
         <v>56</v>
@@ -4363,7 +4242,7 @@
     <row r="62" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E62" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.95314250811525469</v>
+        <v>0.96606045939414131</v>
       </c>
       <c r="F62">
         <v>57</v>
@@ -4392,7 +4271,7 @@
     <row r="63" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E63" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23792840821063677</v>
+        <v>0.7766066134471159</v>
       </c>
       <c r="F63">
         <v>58</v>
@@ -4421,7 +4300,7 @@
     <row r="64" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E64" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78610207821284916</v>
+        <v>0.94766453933334227</v>
       </c>
       <c r="F64">
         <v>59</v>
@@ -4450,7 +4329,7 @@
     <row r="65" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E65" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26254256272022025</v>
+        <v>-0.64359432247293191</v>
       </c>
       <c r="F65">
         <v>60</v>
@@ -4701,18 +4580,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4735,14 +4614,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31965BD6-C292-449A-A97A-E7E72DCB8018}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{402D1E90-AF6A-4728-95AF-C6F39289CFA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4757,4 +4628,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31965BD6-C292-449A-A97A-E7E72DCB8018}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>